<commit_message>
Done with parallel text
</commit_message>
<xml_diff>
--- a/Adhola Proverbs.xlsx
+++ b/Adhola Proverbs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <r>
       <rPr>
@@ -175,9 +175,6 @@
   </si>
   <si>
     <t>I hail government proposal to have local languages used and taught in early childhood at schools.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The saying 'use it or lose it' is pertinent. </t>
   </si>
   <si>
     <t>Failure to use our local language of Dhopadhola may lead to its extinction</t>
@@ -232,10 +229,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -533,225 +533,223 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="93" customWidth="1"/>
-    <col min="2" max="2" width="52.85546875" customWidth="1"/>
+    <col min="1" max="1" width="93" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="30">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:2" ht="30">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:2" ht="30">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:2" ht="30">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:2" ht="30">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:2" ht="30">
+      <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:2" ht="30">
+      <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:2" ht="30">
+      <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:2" ht="30">
+      <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:2" ht="30">
+      <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:2" ht="45">
+      <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="1" t="s">
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" ht="30">
+      <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="1" t="s">
+      <c r="B23" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="30">
+      <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:2" ht="30">
+      <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="1" t="s">
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" ht="30">
+      <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:2" ht="30">
+      <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="1"/>
+      <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:2" ht="30">
+      <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:2" ht="30">
+      <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:2" ht="30">
+      <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:1" ht="30">
+      <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 160 from Facebook
</commit_message>
<xml_diff>
--- a/Adhola Proverbs.xlsx
+++ b/Adhola Proverbs.xlsx
@@ -14,12 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <r>
       <rPr>
         <sz val="11.5"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">Nywoli ber, miyin ichamo gima </t>
     </r>
@@ -27,6 +28,7 @@
       <rPr>
         <sz val="11.5"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>di ikibilo</t>
     </r>
@@ -72,6 +74,7 @@
       <rPr>
         <sz val="11.5"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">Jopadhola jowotan </t>
     </r>
@@ -79,6 +82,7 @@
       <rPr>
         <sz val="11.5"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>ma thurin gimawiloka.</t>
     </r>
@@ -163,6 +167,7 @@
       <rPr>
         <sz val="11.5"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">children chose to marry outside the Adhola tribe. </t>
     </r>
@@ -184,13 +189,31 @@
   </si>
   <si>
     <t>DHOPADHOLAPROVERBS AND SIMILES</t>
+  </si>
+  <si>
+    <t>Achero michiemo iye iweyo chieng baro</t>
+  </si>
+  <si>
+    <t>Cutting the hand that feeds you</t>
+  </si>
+  <si>
+    <t>Achero pamunenwa kiyawi</t>
+  </si>
+  <si>
+    <t>A gift from an intimate friend is never doubted</t>
+  </si>
+  <si>
+    <t>Achero wil</t>
+  </si>
+  <si>
+    <t>scratch by back, and I will scratch yours)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -200,6 +223,13 @@
     <font>
       <sz val="11.5"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF14171A"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -229,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -237,6 +267,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -733,24 +764,48 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:2">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="30">
+    <row r="35" spans="1:2" ht="30">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:2">
       <c r="A36" s="2" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="16.5">
+      <c r="A38" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
submitted the 2nd version
</commit_message>
<xml_diff>
--- a/Adhola Proverbs.xlsx
+++ b/Adhola Proverbs.xlsx
@@ -206,7 +206,7 @@
     <t>Achero wil</t>
   </si>
   <si>
-    <t>scratch by back, and I will scratch yours)</t>
+    <t>scratch by back, and I will scratch yours</t>
   </si>
 </sst>
 </file>
@@ -565,7 +565,7 @@
   <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="A38" sqref="A38:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -810,5 +810,6 @@
     </row>
   </sheetData>
   <pageMargins left="1.25" right="1.25" top="1" bottom="0.79166666666666696" header="0.25" footer="0.25"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>